<commit_message>
Added gannt chart and weekly report
</commit_message>
<xml_diff>
--- a/FALL_22_CLASSES_SEM_1/CSE_534_INFO_ASSUANCE_AND_SECURITY/simple-gantt-chart_ms.xlsx
+++ b/FALL_22_CLASSES_SEM_1/CSE_534_INFO_ASSUANCE_AND_SECURITY/simple-gantt-chart_ms.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Amey\ASU\ASU_MCS\FALL_22_CLASSES_SEM_1\CSE_534_INFO_ASSUANCE_AND_SECURITY\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FA4780E-5796-4CF2-99CD-05EE4ABF96CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5192AA4-3068-4698-8DCB-6520ECFC23F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17,7 +17,7 @@
     <sheet name="About" sheetId="12" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">ProjectSchedule!$1:$39</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">ProjectSchedule!$1:$51</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">ProjectSchedule!$4:$6</definedName>
     <definedName name="task_end" localSheetId="0">ProjectSchedule!$F1</definedName>
     <definedName name="task_progress" localSheetId="0">ProjectSchedule!$D1</definedName>
@@ -77,7 +77,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="68">
   <si>
     <t>Project Start:</t>
   </si>
@@ -191,15 +191,6 @@
     <t>Rohit Vishwanath Badugu, Naveen Aaditya Chitirala</t>
   </si>
   <si>
-    <t>Reasearch Work</t>
-  </si>
-  <si>
-    <t>Project Report annd Weekly Report Work</t>
-  </si>
-  <si>
-    <t>Weekly Report 3</t>
-  </si>
-  <si>
     <t>Use/Applications of ML in IAM Systems</t>
   </si>
   <si>
@@ -225,6 +216,72 @@
   </si>
   <si>
     <t>Exploration of different measures, reasearch papers on topics related to IAM System in Cloud</t>
+  </si>
+  <si>
+    <t>Weekly Report 4</t>
+  </si>
+  <si>
+    <t>Project Report annd Weekly Report Work 4</t>
+  </si>
+  <si>
+    <t>Project Report annd Weekly Report Work 3</t>
+  </si>
+  <si>
+    <t>Project Proposal Finalization</t>
+  </si>
+  <si>
+    <t>Rohit Vishwanath Badugu, Bhavani Priya Kuche</t>
+  </si>
+  <si>
+    <t>Finalizing research Materials</t>
+  </si>
+  <si>
+    <t>Naveen Aaditya Chitirala, Mahita Singamsetty</t>
+  </si>
+  <si>
+    <t>Amey Bhilegaonkar</t>
+  </si>
+  <si>
+    <t>Akash Roshan Mund</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bhavani Priya Kuche </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rohit Vishwanath Badugu </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Naveen Aaditya Chitirala </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kasi Kishore Ravuri </t>
+  </si>
+  <si>
+    <t>Mahita Singamsetty</t>
+  </si>
+  <si>
+    <t>In depth study and report making - Paper 1</t>
+  </si>
+  <si>
+    <t>In depth study and report making - Paper 2</t>
+  </si>
+  <si>
+    <t>In depth study and report making - Paper 3</t>
+  </si>
+  <si>
+    <t>In depth study and report making - Paper 4</t>
+  </si>
+  <si>
+    <t>In depth study and report making - Paper 5</t>
+  </si>
+  <si>
+    <t>In depth study and report making - Paper 6</t>
+  </si>
+  <si>
+    <t>In depth study and report making - Paper 7</t>
+  </si>
+  <si>
+    <t>Review of Reports of each member from the in-depth analysis</t>
   </si>
 </sst>
 </file>
@@ -237,7 +294,7 @@
     <numFmt numFmtId="166" formatCode="mmm\ d\,\ yyyy"/>
     <numFmt numFmtId="167" formatCode="d"/>
   </numFmts>
-  <fonts count="26" x14ac:knownFonts="1">
+  <fonts count="27" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -418,6 +475,12 @@
       <color theme="4" tint="-0.249977111117893"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="12">
@@ -841,77 +904,77 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="4" fillId="5" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="4" fillId="11" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="11" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="11" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="5" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="5" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="5" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="5" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="4" fillId="5" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="4" fillId="11" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="11" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="11" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1487,11 +1550,11 @@
   <sheetPr codeName="Sheet1">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:BL41"/>
+  <dimension ref="A1:BL53"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" showRuler="0" zoomScale="56" zoomScaleNormal="100" zoomScalePageLayoutView="70" workbookViewId="0">
-      <pane ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AL20" sqref="AL20"/>
+    <sheetView showGridLines="0" tabSelected="1" showRuler="0" zoomScale="64" zoomScaleNormal="100" zoomScalePageLayoutView="70" workbookViewId="0">
+      <pane ySplit="6" topLeftCell="A24" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1518,24 +1581,24 @@
       <c r="F1" s="69"/>
       <c r="H1" s="2"/>
       <c r="I1" s="8"/>
-      <c r="J1" s="79"/>
-      <c r="K1" s="79"/>
-      <c r="L1" s="79"/>
-      <c r="M1" s="79"/>
-      <c r="N1" s="79"/>
-      <c r="O1" s="79"/>
-      <c r="P1" s="79"/>
-      <c r="Q1" s="79"/>
-      <c r="R1" s="79"/>
-      <c r="S1" s="79"/>
-      <c r="T1" s="79"/>
-      <c r="U1" s="79"/>
-      <c r="V1" s="79"/>
-      <c r="W1" s="79"/>
-      <c r="X1" s="79"/>
-      <c r="Y1" s="79"/>
-      <c r="Z1" s="79"/>
-      <c r="AA1" s="79"/>
+      <c r="J1" s="92"/>
+      <c r="K1" s="92"/>
+      <c r="L1" s="92"/>
+      <c r="M1" s="92"/>
+      <c r="N1" s="92"/>
+      <c r="O1" s="92"/>
+      <c r="P1" s="92"/>
+      <c r="Q1" s="92"/>
+      <c r="R1" s="92"/>
+      <c r="S1" s="92"/>
+      <c r="T1" s="92"/>
+      <c r="U1" s="92"/>
+      <c r="V1" s="92"/>
+      <c r="W1" s="92"/>
+      <c r="X1" s="92"/>
+      <c r="Y1" s="92"/>
+      <c r="Z1" s="92"/>
+      <c r="AA1" s="92"/>
     </row>
     <row r="2" spans="1:64" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B2" s="9" t="s">
@@ -1544,22 +1607,22 @@
       <c r="D2" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="E2" s="74">
+      <c r="E2" s="96">
         <v>44805</v>
       </c>
-      <c r="F2" s="75"/>
+      <c r="F2" s="97"/>
     </row>
     <row r="3" spans="1:64" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B3" s="9" t="s">
-        <v>39</v>
+        <v>46</v>
       </c>
       <c r="D3" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="E3" s="74">
+      <c r="E3" s="96">
         <v>44864</v>
       </c>
-      <c r="F3" s="75"/>
+      <c r="F3" s="97"/>
     </row>
     <row r="4" spans="1:64" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D4" s="6" t="s">
@@ -1568,86 +1631,86 @@
       <c r="E4" s="7">
         <v>1</v>
       </c>
-      <c r="I4" s="76">
+      <c r="I4" s="93">
         <f>I5</f>
         <v>44802</v>
       </c>
-      <c r="J4" s="77"/>
-      <c r="K4" s="77"/>
-      <c r="L4" s="77"/>
-      <c r="M4" s="77"/>
-      <c r="N4" s="77"/>
-      <c r="O4" s="78"/>
-      <c r="P4" s="76">
+      <c r="J4" s="94"/>
+      <c r="K4" s="94"/>
+      <c r="L4" s="94"/>
+      <c r="M4" s="94"/>
+      <c r="N4" s="94"/>
+      <c r="O4" s="95"/>
+      <c r="P4" s="93">
         <f>P5</f>
         <v>44809</v>
       </c>
-      <c r="Q4" s="77"/>
-      <c r="R4" s="77"/>
-      <c r="S4" s="77"/>
-      <c r="T4" s="77"/>
-      <c r="U4" s="77"/>
-      <c r="V4" s="78"/>
-      <c r="W4" s="76">
+      <c r="Q4" s="94"/>
+      <c r="R4" s="94"/>
+      <c r="S4" s="94"/>
+      <c r="T4" s="94"/>
+      <c r="U4" s="94"/>
+      <c r="V4" s="95"/>
+      <c r="W4" s="93">
         <f>W5</f>
         <v>44816</v>
       </c>
-      <c r="X4" s="77"/>
-      <c r="Y4" s="77"/>
-      <c r="Z4" s="77"/>
-      <c r="AA4" s="77"/>
-      <c r="AB4" s="77"/>
-      <c r="AC4" s="78"/>
-      <c r="AD4" s="76">
+      <c r="X4" s="94"/>
+      <c r="Y4" s="94"/>
+      <c r="Z4" s="94"/>
+      <c r="AA4" s="94"/>
+      <c r="AB4" s="94"/>
+      <c r="AC4" s="95"/>
+      <c r="AD4" s="93">
         <f>AD5</f>
         <v>44823</v>
       </c>
-      <c r="AE4" s="77"/>
-      <c r="AF4" s="77"/>
-      <c r="AG4" s="77"/>
-      <c r="AH4" s="77"/>
-      <c r="AI4" s="77"/>
-      <c r="AJ4" s="78"/>
-      <c r="AK4" s="76">
+      <c r="AE4" s="94"/>
+      <c r="AF4" s="94"/>
+      <c r="AG4" s="94"/>
+      <c r="AH4" s="94"/>
+      <c r="AI4" s="94"/>
+      <c r="AJ4" s="95"/>
+      <c r="AK4" s="93">
         <f>AK5</f>
         <v>44830</v>
       </c>
-      <c r="AL4" s="77"/>
-      <c r="AM4" s="77"/>
-      <c r="AN4" s="77"/>
-      <c r="AO4" s="77"/>
-      <c r="AP4" s="77"/>
-      <c r="AQ4" s="78"/>
-      <c r="AR4" s="76">
+      <c r="AL4" s="94"/>
+      <c r="AM4" s="94"/>
+      <c r="AN4" s="94"/>
+      <c r="AO4" s="94"/>
+      <c r="AP4" s="94"/>
+      <c r="AQ4" s="95"/>
+      <c r="AR4" s="93">
         <f>AR5</f>
         <v>44837</v>
       </c>
-      <c r="AS4" s="77"/>
-      <c r="AT4" s="77"/>
-      <c r="AU4" s="77"/>
-      <c r="AV4" s="77"/>
-      <c r="AW4" s="77"/>
-      <c r="AX4" s="78"/>
-      <c r="AY4" s="76">
+      <c r="AS4" s="94"/>
+      <c r="AT4" s="94"/>
+      <c r="AU4" s="94"/>
+      <c r="AV4" s="94"/>
+      <c r="AW4" s="94"/>
+      <c r="AX4" s="95"/>
+      <c r="AY4" s="93">
         <f>AY5</f>
         <v>44844</v>
       </c>
-      <c r="AZ4" s="77"/>
-      <c r="BA4" s="77"/>
-      <c r="BB4" s="77"/>
-      <c r="BC4" s="77"/>
-      <c r="BD4" s="77"/>
-      <c r="BE4" s="78"/>
-      <c r="BF4" s="76">
+      <c r="AZ4" s="94"/>
+      <c r="BA4" s="94"/>
+      <c r="BB4" s="94"/>
+      <c r="BC4" s="94"/>
+      <c r="BD4" s="94"/>
+      <c r="BE4" s="95"/>
+      <c r="BF4" s="93">
         <f>BF5</f>
         <v>44851</v>
       </c>
-      <c r="BG4" s="77"/>
-      <c r="BH4" s="77"/>
-      <c r="BI4" s="77"/>
-      <c r="BJ4" s="77"/>
-      <c r="BK4" s="77"/>
-      <c r="BL4" s="78"/>
+      <c r="BG4" s="94"/>
+      <c r="BH4" s="94"/>
+      <c r="BI4" s="94"/>
+      <c r="BJ4" s="94"/>
+      <c r="BK4" s="94"/>
+      <c r="BL4" s="95"/>
     </row>
     <row r="5" spans="1:64" x14ac:dyDescent="0.3">
       <c r="A5" s="6"/>
@@ -2125,13 +2188,13 @@
     </row>
     <row r="7" spans="1:64" s="3" customFormat="1" ht="21.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="18"/>
-      <c r="B7" s="80" t="s">
-        <v>47</v>
-      </c>
-      <c r="C7" s="81"/>
-      <c r="D7" s="82"/>
-      <c r="E7" s="83"/>
-      <c r="F7" s="84"/>
+      <c r="B7" s="74" t="s">
+        <v>44</v>
+      </c>
+      <c r="C7" s="75"/>
+      <c r="D7" s="76"/>
+      <c r="E7" s="77"/>
+      <c r="F7" s="78"/>
       <c r="G7" s="24"/>
       <c r="H7" s="24" t="str">
         <f t="shared" ref="H7:H14" si="6">IF(OR(ISBLANK(task_start),ISBLANK(task_end)),"",task_end-task_start+1)</f>
@@ -2196,19 +2259,19 @@
     </row>
     <row r="8" spans="1:64" s="3" customFormat="1" ht="21.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="18"/>
-      <c r="B8" s="85" t="s">
+      <c r="B8" s="79" t="s">
         <v>24</v>
       </c>
-      <c r="C8" s="86" t="s">
+      <c r="C8" s="80" t="s">
         <v>31</v>
       </c>
-      <c r="D8" s="82">
+      <c r="D8" s="76">
         <v>1</v>
       </c>
-      <c r="E8" s="83">
+      <c r="E8" s="77">
         <v>44805</v>
       </c>
-      <c r="F8" s="84">
+      <c r="F8" s="78">
         <v>44806</v>
       </c>
       <c r="G8" s="24"/>
@@ -2219,8 +2282,8 @@
       <c r="I8" s="55"/>
       <c r="J8" s="55"/>
       <c r="K8" s="55"/>
-      <c r="L8" s="87"/>
-      <c r="M8" s="87"/>
+      <c r="L8" s="81"/>
+      <c r="M8" s="81"/>
       <c r="N8" s="55"/>
       <c r="O8" s="55"/>
       <c r="P8" s="55"/>
@@ -2275,19 +2338,19 @@
     </row>
     <row r="9" spans="1:64" s="3" customFormat="1" ht="21.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="18"/>
-      <c r="B9" s="85" t="s">
+      <c r="B9" s="79" t="s">
         <v>25</v>
       </c>
-      <c r="C9" s="86" t="s">
+      <c r="C9" s="80" t="s">
         <v>32</v>
       </c>
-      <c r="D9" s="82">
+      <c r="D9" s="76">
         <v>0.3</v>
       </c>
-      <c r="E9" s="83">
+      <c r="E9" s="77">
         <v>44806</v>
       </c>
-      <c r="F9" s="84">
+      <c r="F9" s="78">
         <v>44809</v>
       </c>
       <c r="G9" s="24"/>
@@ -2354,19 +2417,19 @@
     </row>
     <row r="10" spans="1:64" s="3" customFormat="1" ht="21.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="18"/>
-      <c r="B10" s="85" t="s">
+      <c r="B10" s="79" t="s">
         <v>26</v>
       </c>
-      <c r="C10" s="86" t="s">
+      <c r="C10" s="80" t="s">
         <v>33</v>
       </c>
-      <c r="D10" s="82">
+      <c r="D10" s="76">
         <v>0.8</v>
       </c>
-      <c r="E10" s="83">
+      <c r="E10" s="77">
         <v>44807</v>
       </c>
-      <c r="F10" s="84">
+      <c r="F10" s="78">
         <v>44808</v>
       </c>
       <c r="G10" s="24"/>
@@ -2433,19 +2496,19 @@
     </row>
     <row r="11" spans="1:64" s="3" customFormat="1" ht="21.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="18"/>
-      <c r="B11" s="85" t="s">
+      <c r="B11" s="79" t="s">
         <v>27</v>
       </c>
-      <c r="C11" s="86" t="s">
+      <c r="C11" s="80" t="s">
         <v>36</v>
       </c>
-      <c r="D11" s="82">
+      <c r="D11" s="76">
         <v>0.6</v>
       </c>
-      <c r="E11" s="83">
+      <c r="E11" s="77">
         <v>44808</v>
       </c>
-      <c r="F11" s="84">
+      <c r="F11" s="78">
         <v>44809</v>
       </c>
       <c r="G11" s="24"/>
@@ -2512,19 +2575,19 @@
     </row>
     <row r="12" spans="1:64" s="3" customFormat="1" ht="21.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="18"/>
-      <c r="B12" s="85" t="s">
+      <c r="B12" s="79" t="s">
         <v>28</v>
       </c>
-      <c r="C12" s="86" t="s">
+      <c r="C12" s="80" t="s">
         <v>34</v>
       </c>
-      <c r="D12" s="82">
+      <c r="D12" s="76">
         <v>0.5</v>
       </c>
-      <c r="E12" s="83">
+      <c r="E12" s="77">
         <v>44809</v>
       </c>
-      <c r="F12" s="84">
+      <c r="F12" s="78">
         <v>44812</v>
       </c>
       <c r="G12" s="24"/>
@@ -2591,19 +2654,19 @@
     </row>
     <row r="13" spans="1:64" s="3" customFormat="1" ht="21.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="18"/>
-      <c r="B13" s="85" t="s">
+      <c r="B13" s="79" t="s">
         <v>29</v>
       </c>
-      <c r="C13" s="86" t="s">
+      <c r="C13" s="80" t="s">
         <v>34</v>
       </c>
-      <c r="D13" s="82">
+      <c r="D13" s="76">
         <v>1</v>
       </c>
-      <c r="E13" s="83">
+      <c r="E13" s="77">
         <v>44810</v>
       </c>
-      <c r="F13" s="84">
+      <c r="F13" s="78">
         <v>44812</v>
       </c>
       <c r="G13" s="24"/>
@@ -2667,19 +2730,19 @@
     </row>
     <row r="14" spans="1:64" s="3" customFormat="1" ht="21.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A14" s="18"/>
-      <c r="B14" s="85" t="s">
+      <c r="B14" s="79" t="s">
         <v>30</v>
       </c>
-      <c r="C14" s="86" t="s">
+      <c r="C14" s="80" t="s">
         <v>34</v>
       </c>
-      <c r="D14" s="82">
+      <c r="D14" s="76">
         <v>1</v>
       </c>
-      <c r="E14" s="83">
+      <c r="E14" s="77">
         <v>44811</v>
       </c>
-      <c r="F14" s="84">
+      <c r="F14" s="78">
         <v>44812</v>
       </c>
       <c r="G14" s="24"/>
@@ -2753,7 +2816,7 @@
       <c r="F15" s="23"/>
       <c r="G15" s="24"/>
       <c r="H15" s="24" t="str">
-        <f t="shared" ref="H15:H39" si="7">IF(OR(ISBLANK(task_start),ISBLANK(task_end)),"",task_end-task_start+1)</f>
+        <f t="shared" ref="H15:H51" si="7">IF(OR(ISBLANK(task_start),ISBLANK(task_end)),"",task_end-task_start+1)</f>
         <v/>
       </c>
       <c r="I15" s="55"/>
@@ -2816,7 +2879,7 @@
     <row r="16" spans="1:64" s="3" customFormat="1" ht="21.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A16" s="18"/>
       <c r="B16" s="25" t="s">
-        <v>38</v>
+        <v>48</v>
       </c>
       <c r="C16" s="26"/>
       <c r="D16" s="27"/>
@@ -3434,81 +3497,81 @@
       <c r="BK23" s="55"/>
       <c r="BL23" s="55"/>
     </row>
-    <row r="24" spans="1:64" s="96" customFormat="1" ht="21.6" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="88"/>
-      <c r="B24" s="89"/>
-      <c r="C24" s="90"/>
-      <c r="D24" s="91"/>
-      <c r="E24" s="92"/>
-      <c r="F24" s="93"/>
-      <c r="G24" s="94"/>
-      <c r="H24" s="94"/>
-      <c r="I24" s="95"/>
-      <c r="J24" s="95"/>
-      <c r="K24" s="95"/>
-      <c r="L24" s="95"/>
-      <c r="M24" s="95"/>
-      <c r="N24" s="95"/>
-      <c r="O24" s="95"/>
-      <c r="P24" s="95"/>
-      <c r="Q24" s="95"/>
-      <c r="R24" s="95"/>
-      <c r="S24" s="95"/>
-      <c r="T24" s="95"/>
-      <c r="U24" s="95"/>
-      <c r="V24" s="95"/>
-      <c r="W24" s="95"/>
-      <c r="X24" s="95"/>
-      <c r="Y24" s="95"/>
-      <c r="Z24" s="95"/>
-      <c r="AA24" s="95"/>
-      <c r="AB24" s="95"/>
-      <c r="AC24" s="95"/>
-      <c r="AD24" s="95"/>
-      <c r="AE24" s="95"/>
-      <c r="AF24" s="95"/>
-      <c r="AG24" s="95"/>
-      <c r="AH24" s="95"/>
-      <c r="AI24" s="95"/>
-      <c r="AJ24" s="95"/>
-      <c r="AK24" s="95"/>
-      <c r="AL24" s="95"/>
-      <c r="AM24" s="95"/>
-      <c r="AN24" s="95"/>
-      <c r="AO24" s="95"/>
-      <c r="AP24" s="95"/>
-      <c r="AQ24" s="95"/>
-      <c r="AR24" s="95"/>
-      <c r="AS24" s="95"/>
-      <c r="AT24" s="95"/>
-      <c r="AU24" s="95"/>
-      <c r="AV24" s="95"/>
-      <c r="AW24" s="95"/>
-      <c r="AX24" s="95"/>
-      <c r="AY24" s="95"/>
-      <c r="AZ24" s="95"/>
-      <c r="BA24" s="95"/>
-      <c r="BB24" s="95"/>
-      <c r="BC24" s="95"/>
-      <c r="BD24" s="95"/>
-      <c r="BE24" s="95"/>
-      <c r="BF24" s="95"/>
-      <c r="BG24" s="95"/>
-      <c r="BH24" s="95"/>
-      <c r="BI24" s="95"/>
-      <c r="BJ24" s="95"/>
-      <c r="BK24" s="95"/>
-      <c r="BL24" s="95"/>
+    <row r="24" spans="1:64" s="3" customFormat="1" ht="21.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A24" s="18"/>
+      <c r="B24" s="30"/>
+      <c r="C24" s="31"/>
+      <c r="D24" s="32"/>
+      <c r="E24" s="33"/>
+      <c r="F24" s="34"/>
+      <c r="G24" s="24"/>
+      <c r="H24" s="24"/>
+      <c r="I24" s="55"/>
+      <c r="J24" s="55"/>
+      <c r="K24" s="55"/>
+      <c r="L24" s="55"/>
+      <c r="M24" s="55"/>
+      <c r="N24" s="55"/>
+      <c r="O24" s="55"/>
+      <c r="P24" s="55"/>
+      <c r="Q24" s="55"/>
+      <c r="R24" s="55"/>
+      <c r="S24" s="55"/>
+      <c r="T24" s="55"/>
+      <c r="U24" s="55"/>
+      <c r="V24" s="55"/>
+      <c r="W24" s="55"/>
+      <c r="X24" s="55"/>
+      <c r="Y24" s="55"/>
+      <c r="Z24" s="55"/>
+      <c r="AA24" s="55"/>
+      <c r="AB24" s="55"/>
+      <c r="AC24" s="55"/>
+      <c r="AD24" s="55"/>
+      <c r="AE24" s="55"/>
+      <c r="AF24" s="55"/>
+      <c r="AG24" s="55"/>
+      <c r="AH24" s="55"/>
+      <c r="AI24" s="55"/>
+      <c r="AJ24" s="55"/>
+      <c r="AK24" s="55"/>
+      <c r="AL24" s="55"/>
+      <c r="AM24" s="55"/>
+      <c r="AN24" s="55"/>
+      <c r="AO24" s="55"/>
+      <c r="AP24" s="55"/>
+      <c r="AQ24" s="55"/>
+      <c r="AR24" s="55"/>
+      <c r="AS24" s="55"/>
+      <c r="AT24" s="55"/>
+      <c r="AU24" s="55"/>
+      <c r="AV24" s="55"/>
+      <c r="AW24" s="55"/>
+      <c r="AX24" s="55"/>
+      <c r="AY24" s="55"/>
+      <c r="AZ24" s="55"/>
+      <c r="BA24" s="55"/>
+      <c r="BB24" s="55"/>
+      <c r="BC24" s="55"/>
+      <c r="BD24" s="55"/>
+      <c r="BE24" s="55"/>
+      <c r="BF24" s="55"/>
+      <c r="BG24" s="55"/>
+      <c r="BH24" s="55"/>
+      <c r="BI24" s="55"/>
+      <c r="BJ24" s="55"/>
+      <c r="BK24" s="55"/>
+      <c r="BL24" s="55"/>
     </row>
     <row r="25" spans="1:64" s="3" customFormat="1" ht="21.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A25" s="18"/>
-      <c r="B25" s="35" t="s">
-        <v>37</v>
-      </c>
-      <c r="C25" s="36"/>
-      <c r="D25" s="37"/>
-      <c r="E25" s="38"/>
-      <c r="F25" s="39"/>
+      <c r="B25" s="45" t="s">
+        <v>47</v>
+      </c>
+      <c r="C25" s="46"/>
+      <c r="D25" s="47"/>
+      <c r="E25" s="48"/>
+      <c r="F25" s="49"/>
       <c r="G25" s="24"/>
       <c r="H25" s="24" t="str">
         <f t="shared" si="7"/>
@@ -3573,23 +3636,25 @@
     </row>
     <row r="26" spans="1:64" s="3" customFormat="1" ht="21.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A26" s="18"/>
-      <c r="B26" s="40" t="s">
-        <v>40</v>
-      </c>
-      <c r="C26" s="41" t="s">
-        <v>45</v>
-      </c>
-      <c r="D26" s="42"/>
-      <c r="E26" s="43">
-        <v>44805</v>
-      </c>
-      <c r="F26" s="44">
-        <v>44854</v>
+      <c r="B26" s="50" t="s">
+        <v>49</v>
+      </c>
+      <c r="C26" s="51" t="s">
+        <v>50</v>
+      </c>
+      <c r="D26" s="52">
+        <v>1</v>
+      </c>
+      <c r="E26" s="53">
+        <v>44819</v>
+      </c>
+      <c r="F26" s="54">
+        <v>44826</v>
       </c>
       <c r="G26" s="24"/>
       <c r="H26" s="24">
         <f t="shared" si="7"/>
-        <v>50</v>
+        <v>8</v>
       </c>
       <c r="I26" s="55"/>
       <c r="J26" s="55"/>
@@ -3650,23 +3715,25 @@
     </row>
     <row r="27" spans="1:64" s="3" customFormat="1" ht="21.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A27" s="18"/>
-      <c r="B27" s="40" t="s">
-        <v>41</v>
-      </c>
-      <c r="C27" s="41" t="s">
-        <v>45</v>
-      </c>
-      <c r="D27" s="42"/>
-      <c r="E27" s="43">
-        <v>44806</v>
-      </c>
-      <c r="F27" s="44">
-        <v>44854</v>
+      <c r="B27" s="50" t="s">
+        <v>51</v>
+      </c>
+      <c r="C27" s="51" t="s">
+        <v>52</v>
+      </c>
+      <c r="D27" s="52">
+        <v>1</v>
+      </c>
+      <c r="E27" s="53">
+        <v>44821</v>
+      </c>
+      <c r="F27" s="54">
+        <v>44826</v>
       </c>
       <c r="G27" s="24"/>
       <c r="H27" s="24">
         <f t="shared" si="7"/>
-        <v>49</v>
+        <v>6</v>
       </c>
       <c r="I27" s="55"/>
       <c r="J27" s="55"/>
@@ -3680,8 +3747,8 @@
       <c r="R27" s="55"/>
       <c r="S27" s="55"/>
       <c r="T27" s="55"/>
-      <c r="U27" s="56"/>
-      <c r="V27" s="56"/>
+      <c r="U27" s="55"/>
+      <c r="V27" s="55"/>
       <c r="W27" s="55"/>
       <c r="X27" s="55"/>
       <c r="Y27" s="55"/>
@@ -3727,23 +3794,25 @@
     </row>
     <row r="28" spans="1:64" s="3" customFormat="1" ht="21.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A28" s="18"/>
-      <c r="B28" s="40" t="s">
-        <v>42</v>
-      </c>
-      <c r="C28" s="41" t="s">
-        <v>45</v>
-      </c>
-      <c r="D28" s="42"/>
-      <c r="E28" s="43">
-        <v>44807</v>
-      </c>
-      <c r="F28" s="44">
-        <v>44854</v>
+      <c r="B28" s="50" t="s">
+        <v>60</v>
+      </c>
+      <c r="C28" s="51" t="s">
+        <v>53</v>
+      </c>
+      <c r="D28" s="52">
+        <v>0.1</v>
+      </c>
+      <c r="E28" s="53">
+        <v>44823</v>
+      </c>
+      <c r="F28" s="54">
+        <v>44831</v>
       </c>
       <c r="G28" s="24"/>
       <c r="H28" s="24">
         <f t="shared" si="7"/>
-        <v>48</v>
+        <v>9</v>
       </c>
       <c r="I28" s="55"/>
       <c r="J28" s="55"/>
@@ -3804,23 +3873,25 @@
     </row>
     <row r="29" spans="1:64" s="3" customFormat="1" ht="21.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A29" s="18"/>
-      <c r="B29" s="40" t="s">
-        <v>43</v>
-      </c>
-      <c r="C29" s="41" t="s">
-        <v>45</v>
-      </c>
-      <c r="D29" s="42"/>
-      <c r="E29" s="43">
-        <v>44808</v>
-      </c>
-      <c r="F29" s="44">
-        <v>44854</v>
+      <c r="B29" s="50" t="s">
+        <v>61</v>
+      </c>
+      <c r="C29" s="51" t="s">
+        <v>54</v>
+      </c>
+      <c r="D29" s="52">
+        <v>0.1</v>
+      </c>
+      <c r="E29" s="53">
+        <v>44823</v>
+      </c>
+      <c r="F29" s="54">
+        <v>44831</v>
       </c>
       <c r="G29" s="24"/>
       <c r="H29" s="24">
         <f t="shared" si="7"/>
-        <v>47</v>
+        <v>9</v>
       </c>
       <c r="I29" s="55"/>
       <c r="J29" s="55"/>
@@ -3838,7 +3909,7 @@
       <c r="V29" s="55"/>
       <c r="W29" s="55"/>
       <c r="X29" s="55"/>
-      <c r="Y29" s="56"/>
+      <c r="Y29" s="55"/>
       <c r="Z29" s="55"/>
       <c r="AA29" s="55"/>
       <c r="AB29" s="55"/>
@@ -3881,21 +3952,26 @@
     </row>
     <row r="30" spans="1:64" s="3" customFormat="1" ht="21.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A30" s="18"/>
-      <c r="B30" s="97" t="s">
-        <v>44</v>
-      </c>
-      <c r="C30" s="41" t="s">
-        <v>45</v>
-      </c>
-      <c r="D30" s="42"/>
-      <c r="E30" s="43">
-        <v>44809</v>
-      </c>
-      <c r="F30" s="44">
-        <v>44854</v>
+      <c r="B30" s="50" t="s">
+        <v>62</v>
+      </c>
+      <c r="C30" s="51" t="s">
+        <v>55</v>
+      </c>
+      <c r="D30" s="52">
+        <v>0.1</v>
+      </c>
+      <c r="E30" s="53">
+        <v>44823</v>
+      </c>
+      <c r="F30" s="54">
+        <v>44831</v>
       </c>
       <c r="G30" s="24"/>
-      <c r="H30" s="24"/>
+      <c r="H30" s="24">
+        <f t="shared" si="7"/>
+        <v>9</v>
+      </c>
       <c r="I30" s="55"/>
       <c r="J30" s="55"/>
       <c r="K30" s="55"/>
@@ -3912,7 +3988,7 @@
       <c r="V30" s="55"/>
       <c r="W30" s="55"/>
       <c r="X30" s="55"/>
-      <c r="Y30" s="56"/>
+      <c r="Y30" s="55"/>
       <c r="Z30" s="55"/>
       <c r="AA30" s="55"/>
       <c r="AB30" s="55"/>
@@ -3953,20 +4029,22 @@
       <c r="BK30" s="55"/>
       <c r="BL30" s="55"/>
     </row>
-    <row r="31" spans="1:64" s="3" customFormat="1" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:64" s="3" customFormat="1" ht="21.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A31" s="18"/>
-      <c r="B31" s="97" t="s">
-        <v>48</v>
-      </c>
-      <c r="C31" s="41" t="s">
-        <v>45</v>
-      </c>
-      <c r="D31" s="42"/>
-      <c r="E31" s="43">
-        <v>44810</v>
-      </c>
-      <c r="F31" s="44">
-        <v>44854</v>
+      <c r="B31" s="50" t="s">
+        <v>63</v>
+      </c>
+      <c r="C31" s="51" t="s">
+        <v>56</v>
+      </c>
+      <c r="D31" s="52">
+        <v>0.1</v>
+      </c>
+      <c r="E31" s="53">
+        <v>44823</v>
+      </c>
+      <c r="F31" s="54">
+        <v>44831</v>
       </c>
       <c r="G31" s="24"/>
       <c r="H31" s="24"/>
@@ -3986,7 +4064,7 @@
       <c r="V31" s="55"/>
       <c r="W31" s="55"/>
       <c r="X31" s="55"/>
-      <c r="Y31" s="56"/>
+      <c r="Y31" s="55"/>
       <c r="Z31" s="55"/>
       <c r="AA31" s="55"/>
       <c r="AB31" s="55"/>
@@ -4029,16 +4107,20 @@
     </row>
     <row r="32" spans="1:64" s="3" customFormat="1" ht="21.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A32" s="18"/>
-      <c r="B32" s="40"/>
-      <c r="C32" s="41" t="s">
-        <v>45</v>
-      </c>
-      <c r="D32" s="42"/>
-      <c r="E32" s="43">
-        <v>44811</v>
-      </c>
-      <c r="F32" s="44">
-        <v>44854</v>
+      <c r="B32" s="50" t="s">
+        <v>64</v>
+      </c>
+      <c r="C32" s="51" t="s">
+        <v>57</v>
+      </c>
+      <c r="D32" s="52">
+        <v>0.1</v>
+      </c>
+      <c r="E32" s="53">
+        <v>44823</v>
+      </c>
+      <c r="F32" s="54">
+        <v>44831</v>
       </c>
       <c r="G32" s="24"/>
       <c r="H32" s="24"/>
@@ -4058,7 +4140,7 @@
       <c r="V32" s="55"/>
       <c r="W32" s="55"/>
       <c r="X32" s="55"/>
-      <c r="Y32" s="56"/>
+      <c r="Y32" s="55"/>
       <c r="Z32" s="55"/>
       <c r="AA32" s="55"/>
       <c r="AB32" s="55"/>
@@ -4099,325 +4181,313 @@
       <c r="BK32" s="55"/>
       <c r="BL32" s="55"/>
     </row>
-    <row r="33" spans="1:64" s="3" customFormat="1" ht="21.6" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A33" s="18"/>
-      <c r="B33" s="40"/>
-      <c r="C33" s="41" t="s">
-        <v>45</v>
-      </c>
-      <c r="D33" s="42"/>
-      <c r="E33" s="43">
-        <v>44812</v>
-      </c>
-      <c r="F33" s="44">
-        <v>44854</v>
-      </c>
-      <c r="G33" s="24"/>
-      <c r="H33" s="24">
-        <f t="shared" si="7"/>
-        <v>43</v>
-      </c>
-      <c r="I33" s="55"/>
-      <c r="J33" s="55"/>
-      <c r="K33" s="55"/>
-      <c r="L33" s="55"/>
-      <c r="M33" s="55"/>
-      <c r="N33" s="55"/>
-      <c r="O33" s="55"/>
-      <c r="P33" s="55"/>
-      <c r="Q33" s="55"/>
-      <c r="R33" s="55"/>
-      <c r="S33" s="55"/>
-      <c r="T33" s="55"/>
-      <c r="U33" s="55"/>
-      <c r="V33" s="55"/>
-      <c r="W33" s="55"/>
-      <c r="X33" s="55"/>
-      <c r="Y33" s="55"/>
-      <c r="Z33" s="55"/>
-      <c r="AA33" s="55"/>
-      <c r="AB33" s="55"/>
-      <c r="AC33" s="55"/>
-      <c r="AD33" s="55"/>
-      <c r="AE33" s="55"/>
-      <c r="AF33" s="55"/>
-      <c r="AG33" s="55"/>
-      <c r="AH33" s="55"/>
-      <c r="AI33" s="55"/>
-      <c r="AJ33" s="55"/>
-      <c r="AK33" s="55"/>
-      <c r="AL33" s="55"/>
-      <c r="AM33" s="55"/>
-      <c r="AN33" s="55"/>
-      <c r="AO33" s="55"/>
-      <c r="AP33" s="55"/>
-      <c r="AQ33" s="55"/>
-      <c r="AR33" s="55"/>
-      <c r="AS33" s="55"/>
-      <c r="AT33" s="55"/>
-      <c r="AU33" s="55"/>
-      <c r="AV33" s="55"/>
-      <c r="AW33" s="55"/>
-      <c r="AX33" s="55"/>
-      <c r="AY33" s="55"/>
-      <c r="AZ33" s="55"/>
-      <c r="BA33" s="55"/>
-      <c r="BB33" s="55"/>
-      <c r="BC33" s="55"/>
-      <c r="BD33" s="55"/>
-      <c r="BE33" s="55"/>
-      <c r="BF33" s="55"/>
-      <c r="BG33" s="55"/>
-      <c r="BH33" s="55"/>
-      <c r="BI33" s="55"/>
-      <c r="BJ33" s="55"/>
-      <c r="BK33" s="55"/>
-      <c r="BL33" s="55"/>
-    </row>
-    <row r="34" spans="1:64" s="3" customFormat="1" ht="21.6" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A34" s="18"/>
-      <c r="B34" s="45" t="s">
-        <v>46</v>
-      </c>
-      <c r="C34" s="46"/>
-      <c r="D34" s="47"/>
-      <c r="E34" s="48"/>
-      <c r="F34" s="49"/>
-      <c r="G34" s="24"/>
-      <c r="H34" s="24" t="str">
+    <row r="33" spans="1:64" s="90" customFormat="1" ht="21.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A33" s="82"/>
+      <c r="B33" s="50" t="s">
+        <v>65</v>
+      </c>
+      <c r="C33" s="51" t="s">
+        <v>58</v>
+      </c>
+      <c r="D33" s="52">
+        <v>0.1</v>
+      </c>
+      <c r="E33" s="53">
+        <v>44823</v>
+      </c>
+      <c r="F33" s="54">
+        <v>44831</v>
+      </c>
+      <c r="G33" s="88"/>
+      <c r="H33" s="88"/>
+      <c r="I33" s="89"/>
+      <c r="J33" s="89"/>
+      <c r="K33" s="89"/>
+      <c r="L33" s="89"/>
+      <c r="M33" s="89"/>
+      <c r="N33" s="89"/>
+      <c r="O33" s="89"/>
+      <c r="P33" s="89"/>
+      <c r="Q33" s="89"/>
+      <c r="R33" s="89"/>
+      <c r="S33" s="89"/>
+      <c r="T33" s="89"/>
+      <c r="U33" s="89"/>
+      <c r="V33" s="89"/>
+      <c r="W33" s="89"/>
+      <c r="X33" s="89"/>
+      <c r="Y33" s="89"/>
+      <c r="Z33" s="89"/>
+      <c r="AA33" s="89"/>
+      <c r="AB33" s="89"/>
+      <c r="AC33" s="89"/>
+      <c r="AD33" s="89"/>
+      <c r="AE33" s="89"/>
+      <c r="AF33" s="89"/>
+      <c r="AG33" s="89"/>
+      <c r="AH33" s="89"/>
+      <c r="AI33" s="89"/>
+      <c r="AJ33" s="89"/>
+      <c r="AK33" s="89"/>
+      <c r="AL33" s="89"/>
+      <c r="AM33" s="89"/>
+      <c r="AN33" s="89"/>
+      <c r="AO33" s="89"/>
+      <c r="AP33" s="89"/>
+      <c r="AQ33" s="89"/>
+      <c r="AR33" s="89"/>
+      <c r="AS33" s="89"/>
+      <c r="AT33" s="89"/>
+      <c r="AU33" s="89"/>
+      <c r="AV33" s="89"/>
+      <c r="AW33" s="89"/>
+      <c r="AX33" s="89"/>
+      <c r="AY33" s="89"/>
+      <c r="AZ33" s="89"/>
+      <c r="BA33" s="89"/>
+      <c r="BB33" s="89"/>
+      <c r="BC33" s="89"/>
+      <c r="BD33" s="89"/>
+      <c r="BE33" s="89"/>
+      <c r="BF33" s="89"/>
+      <c r="BG33" s="89"/>
+      <c r="BH33" s="89"/>
+      <c r="BI33" s="89"/>
+      <c r="BJ33" s="89"/>
+      <c r="BK33" s="89"/>
+      <c r="BL33" s="89"/>
+    </row>
+    <row r="34" spans="1:64" s="90" customFormat="1" ht="21.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A34" s="82"/>
+      <c r="B34" s="50" t="s">
+        <v>66</v>
+      </c>
+      <c r="C34" s="51" t="s">
+        <v>59</v>
+      </c>
+      <c r="D34" s="52">
+        <v>0.1</v>
+      </c>
+      <c r="E34" s="53">
+        <v>44823</v>
+      </c>
+      <c r="F34" s="54">
+        <v>44831</v>
+      </c>
+      <c r="G34" s="88"/>
+      <c r="H34" s="88"/>
+      <c r="I34" s="89"/>
+      <c r="J34" s="89"/>
+      <c r="K34" s="89"/>
+      <c r="L34" s="89"/>
+      <c r="M34" s="89"/>
+      <c r="N34" s="89"/>
+      <c r="O34" s="89"/>
+      <c r="P34" s="89"/>
+      <c r="Q34" s="89"/>
+      <c r="R34" s="89"/>
+      <c r="S34" s="89"/>
+      <c r="T34" s="89"/>
+      <c r="U34" s="89"/>
+      <c r="V34" s="89"/>
+      <c r="W34" s="89"/>
+      <c r="X34" s="89"/>
+      <c r="Y34" s="89"/>
+      <c r="Z34" s="89"/>
+      <c r="AA34" s="89"/>
+      <c r="AB34" s="89"/>
+      <c r="AC34" s="89"/>
+      <c r="AD34" s="89"/>
+      <c r="AE34" s="89"/>
+      <c r="AF34" s="89"/>
+      <c r="AG34" s="89"/>
+      <c r="AH34" s="89"/>
+      <c r="AI34" s="89"/>
+      <c r="AJ34" s="89"/>
+      <c r="AK34" s="89"/>
+      <c r="AL34" s="89"/>
+      <c r="AM34" s="89"/>
+      <c r="AN34" s="89"/>
+      <c r="AO34" s="89"/>
+      <c r="AP34" s="89"/>
+      <c r="AQ34" s="89"/>
+      <c r="AR34" s="89"/>
+      <c r="AS34" s="89"/>
+      <c r="AT34" s="89"/>
+      <c r="AU34" s="89"/>
+      <c r="AV34" s="89"/>
+      <c r="AW34" s="89"/>
+      <c r="AX34" s="89"/>
+      <c r="AY34" s="89"/>
+      <c r="AZ34" s="89"/>
+      <c r="BA34" s="89"/>
+      <c r="BB34" s="89"/>
+      <c r="BC34" s="89"/>
+      <c r="BD34" s="89"/>
+      <c r="BE34" s="89"/>
+      <c r="BF34" s="89"/>
+      <c r="BG34" s="89"/>
+      <c r="BH34" s="89"/>
+      <c r="BI34" s="89"/>
+      <c r="BJ34" s="89"/>
+      <c r="BK34" s="89"/>
+      <c r="BL34" s="89"/>
+    </row>
+    <row r="35" spans="1:64" s="90" customFormat="1" ht="21.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A35" s="82"/>
+      <c r="B35" s="50" t="s">
+        <v>67</v>
+      </c>
+      <c r="C35" s="51" t="s">
+        <v>34</v>
+      </c>
+      <c r="D35" s="52">
+        <v>0</v>
+      </c>
+      <c r="E35" s="53">
+        <v>44831</v>
+      </c>
+      <c r="F35" s="54">
+        <v>44833</v>
+      </c>
+      <c r="G35" s="88"/>
+      <c r="H35" s="88"/>
+      <c r="I35" s="89"/>
+      <c r="J35" s="89"/>
+      <c r="K35" s="89"/>
+      <c r="L35" s="89"/>
+      <c r="M35" s="89"/>
+      <c r="N35" s="89"/>
+      <c r="O35" s="89"/>
+      <c r="P35" s="89"/>
+      <c r="Q35" s="89"/>
+      <c r="R35" s="89"/>
+      <c r="S35" s="89"/>
+      <c r="T35" s="89"/>
+      <c r="U35" s="89"/>
+      <c r="V35" s="89"/>
+      <c r="W35" s="89"/>
+      <c r="X35" s="89"/>
+      <c r="Y35" s="89"/>
+      <c r="Z35" s="89"/>
+      <c r="AA35" s="89"/>
+      <c r="AB35" s="89"/>
+      <c r="AC35" s="89"/>
+      <c r="AD35" s="89"/>
+      <c r="AE35" s="89"/>
+      <c r="AF35" s="89"/>
+      <c r="AG35" s="89"/>
+      <c r="AH35" s="89"/>
+      <c r="AI35" s="89"/>
+      <c r="AJ35" s="89"/>
+      <c r="AK35" s="89"/>
+      <c r="AL35" s="89"/>
+      <c r="AM35" s="89"/>
+      <c r="AN35" s="89"/>
+      <c r="AO35" s="89"/>
+      <c r="AP35" s="89"/>
+      <c r="AQ35" s="89"/>
+      <c r="AR35" s="89"/>
+      <c r="AS35" s="89"/>
+      <c r="AT35" s="89"/>
+      <c r="AU35" s="89"/>
+      <c r="AV35" s="89"/>
+      <c r="AW35" s="89"/>
+      <c r="AX35" s="89"/>
+      <c r="AY35" s="89"/>
+      <c r="AZ35" s="89"/>
+      <c r="BA35" s="89"/>
+      <c r="BB35" s="89"/>
+      <c r="BC35" s="89"/>
+      <c r="BD35" s="89"/>
+      <c r="BE35" s="89"/>
+      <c r="BF35" s="89"/>
+      <c r="BG35" s="89"/>
+      <c r="BH35" s="89"/>
+      <c r="BI35" s="89"/>
+      <c r="BJ35" s="89"/>
+      <c r="BK35" s="89"/>
+      <c r="BL35" s="89"/>
+    </row>
+    <row r="36" spans="1:64" s="90" customFormat="1" ht="21.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A36" s="82"/>
+      <c r="B36" s="83"/>
+      <c r="C36" s="84"/>
+      <c r="D36" s="85"/>
+      <c r="E36" s="86"/>
+      <c r="F36" s="87"/>
+      <c r="G36" s="88"/>
+      <c r="H36" s="88"/>
+      <c r="I36" s="89"/>
+      <c r="J36" s="89"/>
+      <c r="K36" s="89"/>
+      <c r="L36" s="89"/>
+      <c r="M36" s="89"/>
+      <c r="N36" s="89"/>
+      <c r="O36" s="89"/>
+      <c r="P36" s="89"/>
+      <c r="Q36" s="89"/>
+      <c r="R36" s="89"/>
+      <c r="S36" s="89"/>
+      <c r="T36" s="89"/>
+      <c r="U36" s="89"/>
+      <c r="V36" s="89"/>
+      <c r="W36" s="89"/>
+      <c r="X36" s="89"/>
+      <c r="Y36" s="89"/>
+      <c r="Z36" s="89"/>
+      <c r="AA36" s="89"/>
+      <c r="AB36" s="89"/>
+      <c r="AC36" s="89"/>
+      <c r="AD36" s="89"/>
+      <c r="AE36" s="89"/>
+      <c r="AF36" s="89"/>
+      <c r="AG36" s="89"/>
+      <c r="AH36" s="89"/>
+      <c r="AI36" s="89"/>
+      <c r="AJ36" s="89"/>
+      <c r="AK36" s="89"/>
+      <c r="AL36" s="89"/>
+      <c r="AM36" s="89"/>
+      <c r="AN36" s="89"/>
+      <c r="AO36" s="89"/>
+      <c r="AP36" s="89"/>
+      <c r="AQ36" s="89"/>
+      <c r="AR36" s="89"/>
+      <c r="AS36" s="89"/>
+      <c r="AT36" s="89"/>
+      <c r="AU36" s="89"/>
+      <c r="AV36" s="89"/>
+      <c r="AW36" s="89"/>
+      <c r="AX36" s="89"/>
+      <c r="AY36" s="89"/>
+      <c r="AZ36" s="89"/>
+      <c r="BA36" s="89"/>
+      <c r="BB36" s="89"/>
+      <c r="BC36" s="89"/>
+      <c r="BD36" s="89"/>
+      <c r="BE36" s="89"/>
+      <c r="BF36" s="89"/>
+      <c r="BG36" s="89"/>
+      <c r="BH36" s="89"/>
+      <c r="BI36" s="89"/>
+      <c r="BJ36" s="89"/>
+      <c r="BK36" s="89"/>
+      <c r="BL36" s="89"/>
+    </row>
+    <row r="37" spans="1:64" s="3" customFormat="1" ht="21.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A37" s="18"/>
+      <c r="B37" s="35" t="s">
+        <v>47</v>
+      </c>
+      <c r="C37" s="36"/>
+      <c r="D37" s="37"/>
+      <c r="E37" s="38"/>
+      <c r="F37" s="39"/>
+      <c r="G37" s="24"/>
+      <c r="H37" s="24" t="str">
         <f t="shared" si="7"/>
         <v/>
-      </c>
-      <c r="I34" s="55"/>
-      <c r="J34" s="55"/>
-      <c r="K34" s="55"/>
-      <c r="L34" s="55"/>
-      <c r="M34" s="55"/>
-      <c r="N34" s="55"/>
-      <c r="O34" s="55"/>
-      <c r="P34" s="55"/>
-      <c r="Q34" s="55"/>
-      <c r="R34" s="55"/>
-      <c r="S34" s="55"/>
-      <c r="T34" s="55"/>
-      <c r="U34" s="55"/>
-      <c r="V34" s="55"/>
-      <c r="W34" s="55"/>
-      <c r="X34" s="55"/>
-      <c r="Y34" s="55"/>
-      <c r="Z34" s="55"/>
-      <c r="AA34" s="55"/>
-      <c r="AB34" s="55"/>
-      <c r="AC34" s="55"/>
-      <c r="AD34" s="55"/>
-      <c r="AE34" s="55"/>
-      <c r="AF34" s="55"/>
-      <c r="AG34" s="55"/>
-      <c r="AH34" s="55"/>
-      <c r="AI34" s="55"/>
-      <c r="AJ34" s="55"/>
-      <c r="AK34" s="55"/>
-      <c r="AL34" s="55"/>
-      <c r="AM34" s="55"/>
-      <c r="AN34" s="55"/>
-      <c r="AO34" s="55"/>
-      <c r="AP34" s="55"/>
-      <c r="AQ34" s="55"/>
-      <c r="AR34" s="55"/>
-      <c r="AS34" s="55"/>
-      <c r="AT34" s="55"/>
-      <c r="AU34" s="55"/>
-      <c r="AV34" s="55"/>
-      <c r="AW34" s="55"/>
-      <c r="AX34" s="55"/>
-      <c r="AY34" s="55"/>
-      <c r="AZ34" s="55"/>
-      <c r="BA34" s="55"/>
-      <c r="BB34" s="55"/>
-      <c r="BC34" s="55"/>
-      <c r="BD34" s="55"/>
-      <c r="BE34" s="55"/>
-      <c r="BF34" s="55"/>
-      <c r="BG34" s="55"/>
-      <c r="BH34" s="55"/>
-      <c r="BI34" s="55"/>
-      <c r="BJ34" s="55"/>
-      <c r="BK34" s="55"/>
-      <c r="BL34" s="55"/>
-    </row>
-    <row r="35" spans="1:64" s="3" customFormat="1" ht="21.6" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A35" s="18"/>
-      <c r="B35" s="50" t="s">
-        <v>45</v>
-      </c>
-      <c r="C35" s="51" t="s">
-        <v>45</v>
-      </c>
-      <c r="D35" s="52"/>
-      <c r="E35" s="53" t="s">
-        <v>45</v>
-      </c>
-      <c r="F35" s="54" t="s">
-        <v>45</v>
-      </c>
-      <c r="G35" s="24"/>
-      <c r="H35" s="24" t="e">
-        <f t="shared" si="7"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="I35" s="55"/>
-      <c r="J35" s="55"/>
-      <c r="K35" s="55"/>
-      <c r="L35" s="55"/>
-      <c r="M35" s="55"/>
-      <c r="N35" s="55"/>
-      <c r="O35" s="55"/>
-      <c r="P35" s="55"/>
-      <c r="Q35" s="55"/>
-      <c r="R35" s="55"/>
-      <c r="S35" s="55"/>
-      <c r="T35" s="55"/>
-      <c r="U35" s="55"/>
-      <c r="V35" s="55"/>
-      <c r="W35" s="55"/>
-      <c r="X35" s="55"/>
-      <c r="Y35" s="55"/>
-      <c r="Z35" s="55"/>
-      <c r="AA35" s="55"/>
-      <c r="AB35" s="55"/>
-      <c r="AC35" s="55"/>
-      <c r="AD35" s="55"/>
-      <c r="AE35" s="55"/>
-      <c r="AF35" s="55"/>
-      <c r="AG35" s="55"/>
-      <c r="AH35" s="55"/>
-      <c r="AI35" s="55"/>
-      <c r="AJ35" s="55"/>
-      <c r="AK35" s="55"/>
-      <c r="AL35" s="55"/>
-      <c r="AM35" s="55"/>
-      <c r="AN35" s="55"/>
-      <c r="AO35" s="55"/>
-      <c r="AP35" s="55"/>
-      <c r="AQ35" s="55"/>
-      <c r="AR35" s="55"/>
-      <c r="AS35" s="55"/>
-      <c r="AT35" s="55"/>
-      <c r="AU35" s="55"/>
-      <c r="AV35" s="55"/>
-      <c r="AW35" s="55"/>
-      <c r="AX35" s="55"/>
-      <c r="AY35" s="55"/>
-      <c r="AZ35" s="55"/>
-      <c r="BA35" s="55"/>
-      <c r="BB35" s="55"/>
-      <c r="BC35" s="55"/>
-      <c r="BD35" s="55"/>
-      <c r="BE35" s="55"/>
-      <c r="BF35" s="55"/>
-      <c r="BG35" s="55"/>
-      <c r="BH35" s="55"/>
-      <c r="BI35" s="55"/>
-      <c r="BJ35" s="55"/>
-      <c r="BK35" s="55"/>
-      <c r="BL35" s="55"/>
-    </row>
-    <row r="36" spans="1:64" s="3" customFormat="1" ht="21.6" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A36" s="18"/>
-      <c r="B36" s="50" t="s">
-        <v>45</v>
-      </c>
-      <c r="C36" s="51" t="s">
-        <v>45</v>
-      </c>
-      <c r="D36" s="52"/>
-      <c r="E36" s="53" t="s">
-        <v>45</v>
-      </c>
-      <c r="F36" s="54" t="s">
-        <v>45</v>
-      </c>
-      <c r="G36" s="24"/>
-      <c r="H36" s="24" t="e">
-        <f t="shared" si="7"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="I36" s="55"/>
-      <c r="J36" s="55"/>
-      <c r="K36" s="55"/>
-      <c r="L36" s="55"/>
-      <c r="M36" s="55"/>
-      <c r="N36" s="55"/>
-      <c r="O36" s="55"/>
-      <c r="P36" s="55"/>
-      <c r="Q36" s="55"/>
-      <c r="R36" s="55"/>
-      <c r="S36" s="55"/>
-      <c r="T36" s="55"/>
-      <c r="U36" s="55"/>
-      <c r="V36" s="55"/>
-      <c r="W36" s="55"/>
-      <c r="X36" s="55"/>
-      <c r="Y36" s="55"/>
-      <c r="Z36" s="55"/>
-      <c r="AA36" s="55"/>
-      <c r="AB36" s="55"/>
-      <c r="AC36" s="55"/>
-      <c r="AD36" s="55"/>
-      <c r="AE36" s="55"/>
-      <c r="AF36" s="55"/>
-      <c r="AG36" s="55"/>
-      <c r="AH36" s="55"/>
-      <c r="AI36" s="55"/>
-      <c r="AJ36" s="55"/>
-      <c r="AK36" s="55"/>
-      <c r="AL36" s="55"/>
-      <c r="AM36" s="55"/>
-      <c r="AN36" s="55"/>
-      <c r="AO36" s="55"/>
-      <c r="AP36" s="55"/>
-      <c r="AQ36" s="55"/>
-      <c r="AR36" s="55"/>
-      <c r="AS36" s="55"/>
-      <c r="AT36" s="55"/>
-      <c r="AU36" s="55"/>
-      <c r="AV36" s="55"/>
-      <c r="AW36" s="55"/>
-      <c r="AX36" s="55"/>
-      <c r="AY36" s="55"/>
-      <c r="AZ36" s="55"/>
-      <c r="BA36" s="55"/>
-      <c r="BB36" s="55"/>
-      <c r="BC36" s="55"/>
-      <c r="BD36" s="55"/>
-      <c r="BE36" s="55"/>
-      <c r="BF36" s="55"/>
-      <c r="BG36" s="55"/>
-      <c r="BH36" s="55"/>
-      <c r="BI36" s="55"/>
-      <c r="BJ36" s="55"/>
-      <c r="BK36" s="55"/>
-      <c r="BL36" s="55"/>
-    </row>
-    <row r="37" spans="1:64" s="3" customFormat="1" ht="21.6" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A37" s="18"/>
-      <c r="B37" s="50" t="s">
-        <v>45</v>
-      </c>
-      <c r="C37" s="51" t="s">
-        <v>45</v>
-      </c>
-      <c r="D37" s="52"/>
-      <c r="E37" s="53" t="s">
-        <v>45</v>
-      </c>
-      <c r="F37" s="54" t="s">
-        <v>45</v>
-      </c>
-      <c r="G37" s="24"/>
-      <c r="H37" s="24" t="e">
-        <f t="shared" si="7"/>
-        <v>#VALUE!</v>
       </c>
       <c r="I37" s="55"/>
       <c r="J37" s="55"/>
@@ -4478,23 +4548,23 @@
     </row>
     <row r="38" spans="1:64" s="3" customFormat="1" ht="21.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A38" s="18"/>
-      <c r="B38" s="50" t="s">
-        <v>45</v>
-      </c>
-      <c r="C38" s="51" t="s">
-        <v>45</v>
-      </c>
-      <c r="D38" s="52"/>
-      <c r="E38" s="53" t="s">
-        <v>45</v>
-      </c>
-      <c r="F38" s="54" t="s">
-        <v>45</v>
+      <c r="B38" s="40" t="s">
+        <v>37</v>
+      </c>
+      <c r="C38" s="41" t="s">
+        <v>42</v>
+      </c>
+      <c r="D38" s="42"/>
+      <c r="E38" s="43">
+        <v>44805</v>
+      </c>
+      <c r="F38" s="44">
+        <v>44854</v>
       </c>
       <c r="G38" s="24"/>
-      <c r="H38" s="24" t="e">
+      <c r="H38" s="24">
         <f t="shared" si="7"/>
-        <v>#VALUE!</v>
+        <v>50</v>
       </c>
       <c r="I38" s="55"/>
       <c r="J38" s="55"/>
@@ -4555,23 +4625,23 @@
     </row>
     <row r="39" spans="1:64" s="3" customFormat="1" ht="21.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A39" s="18"/>
-      <c r="B39" s="50" t="s">
-        <v>45</v>
-      </c>
-      <c r="C39" s="51" t="s">
-        <v>45</v>
-      </c>
-      <c r="D39" s="52"/>
-      <c r="E39" s="53" t="s">
-        <v>45</v>
-      </c>
-      <c r="F39" s="54" t="s">
-        <v>45</v>
+      <c r="B39" s="40" t="s">
+        <v>38</v>
+      </c>
+      <c r="C39" s="41" t="s">
+        <v>42</v>
+      </c>
+      <c r="D39" s="42"/>
+      <c r="E39" s="43">
+        <v>44806</v>
+      </c>
+      <c r="F39" s="44">
+        <v>44854</v>
       </c>
       <c r="G39" s="24"/>
-      <c r="H39" s="24" t="e">
+      <c r="H39" s="24">
         <f t="shared" si="7"/>
-        <v>#VALUE!</v>
+        <v>49</v>
       </c>
       <c r="I39" s="55"/>
       <c r="J39" s="55"/>
@@ -4585,8 +4655,8 @@
       <c r="R39" s="55"/>
       <c r="S39" s="55"/>
       <c r="T39" s="55"/>
-      <c r="U39" s="55"/>
-      <c r="V39" s="55"/>
+      <c r="U39" s="56"/>
+      <c r="V39" s="56"/>
       <c r="W39" s="55"/>
       <c r="X39" s="55"/>
       <c r="Y39" s="55"/>
@@ -4630,28 +4700,934 @@
       <c r="BK39" s="55"/>
       <c r="BL39" s="55"/>
     </row>
-    <row r="40" spans="1:64" x14ac:dyDescent="0.3">
-      <c r="B40" s="72"/>
-      <c r="C40" s="17"/>
-    </row>
-    <row r="41" spans="1:64" x14ac:dyDescent="0.3">
-      <c r="B41" s="71"/>
+    <row r="40" spans="1:64" s="3" customFormat="1" ht="21.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A40" s="18"/>
+      <c r="B40" s="40" t="s">
+        <v>39</v>
+      </c>
+      <c r="C40" s="41" t="s">
+        <v>42</v>
+      </c>
+      <c r="D40" s="42"/>
+      <c r="E40" s="43">
+        <v>44807</v>
+      </c>
+      <c r="F40" s="44">
+        <v>44854</v>
+      </c>
+      <c r="G40" s="24"/>
+      <c r="H40" s="24">
+        <f t="shared" si="7"/>
+        <v>48</v>
+      </c>
+      <c r="I40" s="55"/>
+      <c r="J40" s="55"/>
+      <c r="K40" s="55"/>
+      <c r="L40" s="55"/>
+      <c r="M40" s="55"/>
+      <c r="N40" s="55"/>
+      <c r="O40" s="55"/>
+      <c r="P40" s="55"/>
+      <c r="Q40" s="55"/>
+      <c r="R40" s="55"/>
+      <c r="S40" s="55"/>
+      <c r="T40" s="55"/>
+      <c r="U40" s="55"/>
+      <c r="V40" s="55"/>
+      <c r="W40" s="55"/>
+      <c r="X40" s="55"/>
+      <c r="Y40" s="55"/>
+      <c r="Z40" s="55"/>
+      <c r="AA40" s="55"/>
+      <c r="AB40" s="55"/>
+      <c r="AC40" s="55"/>
+      <c r="AD40" s="55"/>
+      <c r="AE40" s="55"/>
+      <c r="AF40" s="55"/>
+      <c r="AG40" s="55"/>
+      <c r="AH40" s="55"/>
+      <c r="AI40" s="55"/>
+      <c r="AJ40" s="55"/>
+      <c r="AK40" s="55"/>
+      <c r="AL40" s="55"/>
+      <c r="AM40" s="55"/>
+      <c r="AN40" s="55"/>
+      <c r="AO40" s="55"/>
+      <c r="AP40" s="55"/>
+      <c r="AQ40" s="55"/>
+      <c r="AR40" s="55"/>
+      <c r="AS40" s="55"/>
+      <c r="AT40" s="55"/>
+      <c r="AU40" s="55"/>
+      <c r="AV40" s="55"/>
+      <c r="AW40" s="55"/>
+      <c r="AX40" s="55"/>
+      <c r="AY40" s="55"/>
+      <c r="AZ40" s="55"/>
+      <c r="BA40" s="55"/>
+      <c r="BB40" s="55"/>
+      <c r="BC40" s="55"/>
+      <c r="BD40" s="55"/>
+      <c r="BE40" s="55"/>
+      <c r="BF40" s="55"/>
+      <c r="BG40" s="55"/>
+      <c r="BH40" s="55"/>
+      <c r="BI40" s="55"/>
+      <c r="BJ40" s="55"/>
+      <c r="BK40" s="55"/>
+      <c r="BL40" s="55"/>
+    </row>
+    <row r="41" spans="1:64" s="3" customFormat="1" ht="21.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A41" s="18"/>
+      <c r="B41" s="40" t="s">
+        <v>40</v>
+      </c>
+      <c r="C41" s="41" t="s">
+        <v>42</v>
+      </c>
+      <c r="D41" s="42"/>
+      <c r="E41" s="43">
+        <v>44808</v>
+      </c>
+      <c r="F41" s="44">
+        <v>44854</v>
+      </c>
+      <c r="G41" s="24"/>
+      <c r="H41" s="24">
+        <f t="shared" si="7"/>
+        <v>47</v>
+      </c>
+      <c r="I41" s="55"/>
+      <c r="J41" s="55"/>
+      <c r="K41" s="55"/>
+      <c r="L41" s="55"/>
+      <c r="M41" s="55"/>
+      <c r="N41" s="55"/>
+      <c r="O41" s="55"/>
+      <c r="P41" s="55"/>
+      <c r="Q41" s="55"/>
+      <c r="R41" s="55"/>
+      <c r="S41" s="55"/>
+      <c r="T41" s="55"/>
+      <c r="U41" s="55"/>
+      <c r="V41" s="55"/>
+      <c r="W41" s="55"/>
+      <c r="X41" s="55"/>
+      <c r="Y41" s="56"/>
+      <c r="Z41" s="55"/>
+      <c r="AA41" s="55"/>
+      <c r="AB41" s="55"/>
+      <c r="AC41" s="55"/>
+      <c r="AD41" s="55"/>
+      <c r="AE41" s="55"/>
+      <c r="AF41" s="55"/>
+      <c r="AG41" s="55"/>
+      <c r="AH41" s="55"/>
+      <c r="AI41" s="55"/>
+      <c r="AJ41" s="55"/>
+      <c r="AK41" s="55"/>
+      <c r="AL41" s="55"/>
+      <c r="AM41" s="55"/>
+      <c r="AN41" s="55"/>
+      <c r="AO41" s="55"/>
+      <c r="AP41" s="55"/>
+      <c r="AQ41" s="55"/>
+      <c r="AR41" s="55"/>
+      <c r="AS41" s="55"/>
+      <c r="AT41" s="55"/>
+      <c r="AU41" s="55"/>
+      <c r="AV41" s="55"/>
+      <c r="AW41" s="55"/>
+      <c r="AX41" s="55"/>
+      <c r="AY41" s="55"/>
+      <c r="AZ41" s="55"/>
+      <c r="BA41" s="55"/>
+      <c r="BB41" s="55"/>
+      <c r="BC41" s="55"/>
+      <c r="BD41" s="55"/>
+      <c r="BE41" s="55"/>
+      <c r="BF41" s="55"/>
+      <c r="BG41" s="55"/>
+      <c r="BH41" s="55"/>
+      <c r="BI41" s="55"/>
+      <c r="BJ41" s="55"/>
+      <c r="BK41" s="55"/>
+      <c r="BL41" s="55"/>
+    </row>
+    <row r="42" spans="1:64" s="3" customFormat="1" ht="21.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A42" s="18"/>
+      <c r="B42" s="91" t="s">
+        <v>41</v>
+      </c>
+      <c r="C42" s="41" t="s">
+        <v>42</v>
+      </c>
+      <c r="D42" s="42"/>
+      <c r="E42" s="43">
+        <v>44809</v>
+      </c>
+      <c r="F42" s="44">
+        <v>44854</v>
+      </c>
+      <c r="G42" s="24"/>
+      <c r="H42" s="24"/>
+      <c r="I42" s="55"/>
+      <c r="J42" s="55"/>
+      <c r="K42" s="55"/>
+      <c r="L42" s="55"/>
+      <c r="M42" s="55"/>
+      <c r="N42" s="55"/>
+      <c r="O42" s="55"/>
+      <c r="P42" s="55"/>
+      <c r="Q42" s="55"/>
+      <c r="R42" s="55"/>
+      <c r="S42" s="55"/>
+      <c r="T42" s="55"/>
+      <c r="U42" s="55"/>
+      <c r="V42" s="55"/>
+      <c r="W42" s="55"/>
+      <c r="X42" s="55"/>
+      <c r="Y42" s="56"/>
+      <c r="Z42" s="55"/>
+      <c r="AA42" s="55"/>
+      <c r="AB42" s="55"/>
+      <c r="AC42" s="55"/>
+      <c r="AD42" s="55"/>
+      <c r="AE42" s="55"/>
+      <c r="AF42" s="55"/>
+      <c r="AG42" s="55"/>
+      <c r="AH42" s="55"/>
+      <c r="AI42" s="55"/>
+      <c r="AJ42" s="55"/>
+      <c r="AK42" s="55"/>
+      <c r="AL42" s="55"/>
+      <c r="AM42" s="55"/>
+      <c r="AN42" s="55"/>
+      <c r="AO42" s="55"/>
+      <c r="AP42" s="55"/>
+      <c r="AQ42" s="55"/>
+      <c r="AR42" s="55"/>
+      <c r="AS42" s="55"/>
+      <c r="AT42" s="55"/>
+      <c r="AU42" s="55"/>
+      <c r="AV42" s="55"/>
+      <c r="AW42" s="55"/>
+      <c r="AX42" s="55"/>
+      <c r="AY42" s="55"/>
+      <c r="AZ42" s="55"/>
+      <c r="BA42" s="55"/>
+      <c r="BB42" s="55"/>
+      <c r="BC42" s="55"/>
+      <c r="BD42" s="55"/>
+      <c r="BE42" s="55"/>
+      <c r="BF42" s="55"/>
+      <c r="BG42" s="55"/>
+      <c r="BH42" s="55"/>
+      <c r="BI42" s="55"/>
+      <c r="BJ42" s="55"/>
+      <c r="BK42" s="55"/>
+      <c r="BL42" s="55"/>
+    </row>
+    <row r="43" spans="1:64" s="3" customFormat="1" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A43" s="18"/>
+      <c r="B43" s="91" t="s">
+        <v>45</v>
+      </c>
+      <c r="C43" s="41" t="s">
+        <v>42</v>
+      </c>
+      <c r="D43" s="42"/>
+      <c r="E43" s="43">
+        <v>44810</v>
+      </c>
+      <c r="F43" s="44">
+        <v>44854</v>
+      </c>
+      <c r="G43" s="24"/>
+      <c r="H43" s="24"/>
+      <c r="I43" s="55"/>
+      <c r="J43" s="55"/>
+      <c r="K43" s="55"/>
+      <c r="L43" s="55"/>
+      <c r="M43" s="55"/>
+      <c r="N43" s="55"/>
+      <c r="O43" s="55"/>
+      <c r="P43" s="55"/>
+      <c r="Q43" s="55"/>
+      <c r="R43" s="55"/>
+      <c r="S43" s="55"/>
+      <c r="T43" s="55"/>
+      <c r="U43" s="55"/>
+      <c r="V43" s="55"/>
+      <c r="W43" s="55"/>
+      <c r="X43" s="55"/>
+      <c r="Y43" s="56"/>
+      <c r="Z43" s="55"/>
+      <c r="AA43" s="55"/>
+      <c r="AB43" s="55"/>
+      <c r="AC43" s="55"/>
+      <c r="AD43" s="55"/>
+      <c r="AE43" s="55"/>
+      <c r="AF43" s="55"/>
+      <c r="AG43" s="55"/>
+      <c r="AH43" s="55"/>
+      <c r="AI43" s="55"/>
+      <c r="AJ43" s="55"/>
+      <c r="AK43" s="55"/>
+      <c r="AL43" s="55"/>
+      <c r="AM43" s="55"/>
+      <c r="AN43" s="55"/>
+      <c r="AO43" s="55"/>
+      <c r="AP43" s="55"/>
+      <c r="AQ43" s="55"/>
+      <c r="AR43" s="55"/>
+      <c r="AS43" s="55"/>
+      <c r="AT43" s="55"/>
+      <c r="AU43" s="55"/>
+      <c r="AV43" s="55"/>
+      <c r="AW43" s="55"/>
+      <c r="AX43" s="55"/>
+      <c r="AY43" s="55"/>
+      <c r="AZ43" s="55"/>
+      <c r="BA43" s="55"/>
+      <c r="BB43" s="55"/>
+      <c r="BC43" s="55"/>
+      <c r="BD43" s="55"/>
+      <c r="BE43" s="55"/>
+      <c r="BF43" s="55"/>
+      <c r="BG43" s="55"/>
+      <c r="BH43" s="55"/>
+      <c r="BI43" s="55"/>
+      <c r="BJ43" s="55"/>
+      <c r="BK43" s="55"/>
+      <c r="BL43" s="55"/>
+    </row>
+    <row r="44" spans="1:64" s="3" customFormat="1" ht="21.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A44" s="18"/>
+      <c r="B44" s="40"/>
+      <c r="C44" s="41" t="s">
+        <v>42</v>
+      </c>
+      <c r="D44" s="42"/>
+      <c r="E44" s="43">
+        <v>44811</v>
+      </c>
+      <c r="F44" s="44">
+        <v>44854</v>
+      </c>
+      <c r="G44" s="24"/>
+      <c r="H44" s="24"/>
+      <c r="I44" s="55"/>
+      <c r="J44" s="55"/>
+      <c r="K44" s="55"/>
+      <c r="L44" s="55"/>
+      <c r="M44" s="55"/>
+      <c r="N44" s="55"/>
+      <c r="O44" s="55"/>
+      <c r="P44" s="55"/>
+      <c r="Q44" s="55"/>
+      <c r="R44" s="55"/>
+      <c r="S44" s="55"/>
+      <c r="T44" s="55"/>
+      <c r="U44" s="55"/>
+      <c r="V44" s="55"/>
+      <c r="W44" s="55"/>
+      <c r="X44" s="55"/>
+      <c r="Y44" s="56"/>
+      <c r="Z44" s="55"/>
+      <c r="AA44" s="55"/>
+      <c r="AB44" s="55"/>
+      <c r="AC44" s="55"/>
+      <c r="AD44" s="55"/>
+      <c r="AE44" s="55"/>
+      <c r="AF44" s="55"/>
+      <c r="AG44" s="55"/>
+      <c r="AH44" s="55"/>
+      <c r="AI44" s="55"/>
+      <c r="AJ44" s="55"/>
+      <c r="AK44" s="55"/>
+      <c r="AL44" s="55"/>
+      <c r="AM44" s="55"/>
+      <c r="AN44" s="55"/>
+      <c r="AO44" s="55"/>
+      <c r="AP44" s="55"/>
+      <c r="AQ44" s="55"/>
+      <c r="AR44" s="55"/>
+      <c r="AS44" s="55"/>
+      <c r="AT44" s="55"/>
+      <c r="AU44" s="55"/>
+      <c r="AV44" s="55"/>
+      <c r="AW44" s="55"/>
+      <c r="AX44" s="55"/>
+      <c r="AY44" s="55"/>
+      <c r="AZ44" s="55"/>
+      <c r="BA44" s="55"/>
+      <c r="BB44" s="55"/>
+      <c r="BC44" s="55"/>
+      <c r="BD44" s="55"/>
+      <c r="BE44" s="55"/>
+      <c r="BF44" s="55"/>
+      <c r="BG44" s="55"/>
+      <c r="BH44" s="55"/>
+      <c r="BI44" s="55"/>
+      <c r="BJ44" s="55"/>
+      <c r="BK44" s="55"/>
+      <c r="BL44" s="55"/>
+    </row>
+    <row r="45" spans="1:64" s="3" customFormat="1" ht="21.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A45" s="18"/>
+      <c r="B45" s="40"/>
+      <c r="C45" s="41" t="s">
+        <v>42</v>
+      </c>
+      <c r="D45" s="42"/>
+      <c r="E45" s="43">
+        <v>44812</v>
+      </c>
+      <c r="F45" s="44">
+        <v>44854</v>
+      </c>
+      <c r="G45" s="24"/>
+      <c r="H45" s="24">
+        <f t="shared" si="7"/>
+        <v>43</v>
+      </c>
+      <c r="I45" s="55"/>
+      <c r="J45" s="55"/>
+      <c r="K45" s="55"/>
+      <c r="L45" s="55"/>
+      <c r="M45" s="55"/>
+      <c r="N45" s="55"/>
+      <c r="O45" s="55"/>
+      <c r="P45" s="55"/>
+      <c r="Q45" s="55"/>
+      <c r="R45" s="55"/>
+      <c r="S45" s="55"/>
+      <c r="T45" s="55"/>
+      <c r="U45" s="55"/>
+      <c r="V45" s="55"/>
+      <c r="W45" s="55"/>
+      <c r="X45" s="55"/>
+      <c r="Y45" s="55"/>
+      <c r="Z45" s="55"/>
+      <c r="AA45" s="55"/>
+      <c r="AB45" s="55"/>
+      <c r="AC45" s="55"/>
+      <c r="AD45" s="55"/>
+      <c r="AE45" s="55"/>
+      <c r="AF45" s="55"/>
+      <c r="AG45" s="55"/>
+      <c r="AH45" s="55"/>
+      <c r="AI45" s="55"/>
+      <c r="AJ45" s="55"/>
+      <c r="AK45" s="55"/>
+      <c r="AL45" s="55"/>
+      <c r="AM45" s="55"/>
+      <c r="AN45" s="55"/>
+      <c r="AO45" s="55"/>
+      <c r="AP45" s="55"/>
+      <c r="AQ45" s="55"/>
+      <c r="AR45" s="55"/>
+      <c r="AS45" s="55"/>
+      <c r="AT45" s="55"/>
+      <c r="AU45" s="55"/>
+      <c r="AV45" s="55"/>
+      <c r="AW45" s="55"/>
+      <c r="AX45" s="55"/>
+      <c r="AY45" s="55"/>
+      <c r="AZ45" s="55"/>
+      <c r="BA45" s="55"/>
+      <c r="BB45" s="55"/>
+      <c r="BC45" s="55"/>
+      <c r="BD45" s="55"/>
+      <c r="BE45" s="55"/>
+      <c r="BF45" s="55"/>
+      <c r="BG45" s="55"/>
+      <c r="BH45" s="55"/>
+      <c r="BI45" s="55"/>
+      <c r="BJ45" s="55"/>
+      <c r="BK45" s="55"/>
+      <c r="BL45" s="55"/>
+    </row>
+    <row r="46" spans="1:64" s="3" customFormat="1" ht="21.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A46" s="18"/>
+      <c r="B46" s="45" t="s">
+        <v>43</v>
+      </c>
+      <c r="C46" s="46"/>
+      <c r="D46" s="47"/>
+      <c r="E46" s="48"/>
+      <c r="F46" s="49"/>
+      <c r="G46" s="24"/>
+      <c r="H46" s="24" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+      <c r="I46" s="55"/>
+      <c r="J46" s="55"/>
+      <c r="K46" s="55"/>
+      <c r="L46" s="55"/>
+      <c r="M46" s="55"/>
+      <c r="N46" s="55"/>
+      <c r="O46" s="55"/>
+      <c r="P46" s="55"/>
+      <c r="Q46" s="55"/>
+      <c r="R46" s="55"/>
+      <c r="S46" s="55"/>
+      <c r="T46" s="55"/>
+      <c r="U46" s="55"/>
+      <c r="V46" s="55"/>
+      <c r="W46" s="55"/>
+      <c r="X46" s="55"/>
+      <c r="Y46" s="55"/>
+      <c r="Z46" s="55"/>
+      <c r="AA46" s="55"/>
+      <c r="AB46" s="55"/>
+      <c r="AC46" s="55"/>
+      <c r="AD46" s="55"/>
+      <c r="AE46" s="55"/>
+      <c r="AF46" s="55"/>
+      <c r="AG46" s="55"/>
+      <c r="AH46" s="55"/>
+      <c r="AI46" s="55"/>
+      <c r="AJ46" s="55"/>
+      <c r="AK46" s="55"/>
+      <c r="AL46" s="55"/>
+      <c r="AM46" s="55"/>
+      <c r="AN46" s="55"/>
+      <c r="AO46" s="55"/>
+      <c r="AP46" s="55"/>
+      <c r="AQ46" s="55"/>
+      <c r="AR46" s="55"/>
+      <c r="AS46" s="55"/>
+      <c r="AT46" s="55"/>
+      <c r="AU46" s="55"/>
+      <c r="AV46" s="55"/>
+      <c r="AW46" s="55"/>
+      <c r="AX46" s="55"/>
+      <c r="AY46" s="55"/>
+      <c r="AZ46" s="55"/>
+      <c r="BA46" s="55"/>
+      <c r="BB46" s="55"/>
+      <c r="BC46" s="55"/>
+      <c r="BD46" s="55"/>
+      <c r="BE46" s="55"/>
+      <c r="BF46" s="55"/>
+      <c r="BG46" s="55"/>
+      <c r="BH46" s="55"/>
+      <c r="BI46" s="55"/>
+      <c r="BJ46" s="55"/>
+      <c r="BK46" s="55"/>
+      <c r="BL46" s="55"/>
+    </row>
+    <row r="47" spans="1:64" s="3" customFormat="1" ht="21.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A47" s="18"/>
+      <c r="B47" s="50" t="s">
+        <v>42</v>
+      </c>
+      <c r="C47" s="51" t="s">
+        <v>42</v>
+      </c>
+      <c r="D47" s="52"/>
+      <c r="E47" s="53" t="s">
+        <v>42</v>
+      </c>
+      <c r="F47" s="54" t="s">
+        <v>42</v>
+      </c>
+      <c r="G47" s="24"/>
+      <c r="H47" s="24" t="e">
+        <f t="shared" si="7"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="I47" s="55"/>
+      <c r="J47" s="55"/>
+      <c r="K47" s="55"/>
+      <c r="L47" s="55"/>
+      <c r="M47" s="55"/>
+      <c r="N47" s="55"/>
+      <c r="O47" s="55"/>
+      <c r="P47" s="55"/>
+      <c r="Q47" s="55"/>
+      <c r="R47" s="55"/>
+      <c r="S47" s="55"/>
+      <c r="T47" s="55"/>
+      <c r="U47" s="55"/>
+      <c r="V47" s="55"/>
+      <c r="W47" s="55"/>
+      <c r="X47" s="55"/>
+      <c r="Y47" s="55"/>
+      <c r="Z47" s="55"/>
+      <c r="AA47" s="55"/>
+      <c r="AB47" s="55"/>
+      <c r="AC47" s="55"/>
+      <c r="AD47" s="55"/>
+      <c r="AE47" s="55"/>
+      <c r="AF47" s="55"/>
+      <c r="AG47" s="55"/>
+      <c r="AH47" s="55"/>
+      <c r="AI47" s="55"/>
+      <c r="AJ47" s="55"/>
+      <c r="AK47" s="55"/>
+      <c r="AL47" s="55"/>
+      <c r="AM47" s="55"/>
+      <c r="AN47" s="55"/>
+      <c r="AO47" s="55"/>
+      <c r="AP47" s="55"/>
+      <c r="AQ47" s="55"/>
+      <c r="AR47" s="55"/>
+      <c r="AS47" s="55"/>
+      <c r="AT47" s="55"/>
+      <c r="AU47" s="55"/>
+      <c r="AV47" s="55"/>
+      <c r="AW47" s="55"/>
+      <c r="AX47" s="55"/>
+      <c r="AY47" s="55"/>
+      <c r="AZ47" s="55"/>
+      <c r="BA47" s="55"/>
+      <c r="BB47" s="55"/>
+      <c r="BC47" s="55"/>
+      <c r="BD47" s="55"/>
+      <c r="BE47" s="55"/>
+      <c r="BF47" s="55"/>
+      <c r="BG47" s="55"/>
+      <c r="BH47" s="55"/>
+      <c r="BI47" s="55"/>
+      <c r="BJ47" s="55"/>
+      <c r="BK47" s="55"/>
+      <c r="BL47" s="55"/>
+    </row>
+    <row r="48" spans="1:64" s="3" customFormat="1" ht="21.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A48" s="18"/>
+      <c r="B48" s="50" t="s">
+        <v>42</v>
+      </c>
+      <c r="C48" s="51" t="s">
+        <v>42</v>
+      </c>
+      <c r="D48" s="52"/>
+      <c r="E48" s="53" t="s">
+        <v>42</v>
+      </c>
+      <c r="F48" s="54" t="s">
+        <v>42</v>
+      </c>
+      <c r="G48" s="24"/>
+      <c r="H48" s="24" t="e">
+        <f t="shared" si="7"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="I48" s="55"/>
+      <c r="J48" s="55"/>
+      <c r="K48" s="55"/>
+      <c r="L48" s="55"/>
+      <c r="M48" s="55"/>
+      <c r="N48" s="55"/>
+      <c r="O48" s="55"/>
+      <c r="P48" s="55"/>
+      <c r="Q48" s="55"/>
+      <c r="R48" s="55"/>
+      <c r="S48" s="55"/>
+      <c r="T48" s="55"/>
+      <c r="U48" s="55"/>
+      <c r="V48" s="55"/>
+      <c r="W48" s="55"/>
+      <c r="X48" s="55"/>
+      <c r="Y48" s="55"/>
+      <c r="Z48" s="55"/>
+      <c r="AA48" s="55"/>
+      <c r="AB48" s="55"/>
+      <c r="AC48" s="55"/>
+      <c r="AD48" s="55"/>
+      <c r="AE48" s="55"/>
+      <c r="AF48" s="55"/>
+      <c r="AG48" s="55"/>
+      <c r="AH48" s="55"/>
+      <c r="AI48" s="55"/>
+      <c r="AJ48" s="55"/>
+      <c r="AK48" s="55"/>
+      <c r="AL48" s="55"/>
+      <c r="AM48" s="55"/>
+      <c r="AN48" s="55"/>
+      <c r="AO48" s="55"/>
+      <c r="AP48" s="55"/>
+      <c r="AQ48" s="55"/>
+      <c r="AR48" s="55"/>
+      <c r="AS48" s="55"/>
+      <c r="AT48" s="55"/>
+      <c r="AU48" s="55"/>
+      <c r="AV48" s="55"/>
+      <c r="AW48" s="55"/>
+      <c r="AX48" s="55"/>
+      <c r="AY48" s="55"/>
+      <c r="AZ48" s="55"/>
+      <c r="BA48" s="55"/>
+      <c r="BB48" s="55"/>
+      <c r="BC48" s="55"/>
+      <c r="BD48" s="55"/>
+      <c r="BE48" s="55"/>
+      <c r="BF48" s="55"/>
+      <c r="BG48" s="55"/>
+      <c r="BH48" s="55"/>
+      <c r="BI48" s="55"/>
+      <c r="BJ48" s="55"/>
+      <c r="BK48" s="55"/>
+      <c r="BL48" s="55"/>
+    </row>
+    <row r="49" spans="1:64" s="3" customFormat="1" ht="21.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A49" s="18"/>
+      <c r="B49" s="50" t="s">
+        <v>42</v>
+      </c>
+      <c r="C49" s="51" t="s">
+        <v>42</v>
+      </c>
+      <c r="D49" s="52"/>
+      <c r="E49" s="53" t="s">
+        <v>42</v>
+      </c>
+      <c r="F49" s="54" t="s">
+        <v>42</v>
+      </c>
+      <c r="G49" s="24"/>
+      <c r="H49" s="24" t="e">
+        <f t="shared" si="7"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="I49" s="55"/>
+      <c r="J49" s="55"/>
+      <c r="K49" s="55"/>
+      <c r="L49" s="55"/>
+      <c r="M49" s="55"/>
+      <c r="N49" s="55"/>
+      <c r="O49" s="55"/>
+      <c r="P49" s="55"/>
+      <c r="Q49" s="55"/>
+      <c r="R49" s="55"/>
+      <c r="S49" s="55"/>
+      <c r="T49" s="55"/>
+      <c r="U49" s="55"/>
+      <c r="V49" s="55"/>
+      <c r="W49" s="55"/>
+      <c r="X49" s="55"/>
+      <c r="Y49" s="55"/>
+      <c r="Z49" s="55"/>
+      <c r="AA49" s="55"/>
+      <c r="AB49" s="55"/>
+      <c r="AC49" s="55"/>
+      <c r="AD49" s="55"/>
+      <c r="AE49" s="55"/>
+      <c r="AF49" s="55"/>
+      <c r="AG49" s="55"/>
+      <c r="AH49" s="55"/>
+      <c r="AI49" s="55"/>
+      <c r="AJ49" s="55"/>
+      <c r="AK49" s="55"/>
+      <c r="AL49" s="55"/>
+      <c r="AM49" s="55"/>
+      <c r="AN49" s="55"/>
+      <c r="AO49" s="55"/>
+      <c r="AP49" s="55"/>
+      <c r="AQ49" s="55"/>
+      <c r="AR49" s="55"/>
+      <c r="AS49" s="55"/>
+      <c r="AT49" s="55"/>
+      <c r="AU49" s="55"/>
+      <c r="AV49" s="55"/>
+      <c r="AW49" s="55"/>
+      <c r="AX49" s="55"/>
+      <c r="AY49" s="55"/>
+      <c r="AZ49" s="55"/>
+      <c r="BA49" s="55"/>
+      <c r="BB49" s="55"/>
+      <c r="BC49" s="55"/>
+      <c r="BD49" s="55"/>
+      <c r="BE49" s="55"/>
+      <c r="BF49" s="55"/>
+      <c r="BG49" s="55"/>
+      <c r="BH49" s="55"/>
+      <c r="BI49" s="55"/>
+      <c r="BJ49" s="55"/>
+      <c r="BK49" s="55"/>
+      <c r="BL49" s="55"/>
+    </row>
+    <row r="50" spans="1:64" s="3" customFormat="1" ht="21.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A50" s="18"/>
+      <c r="B50" s="50" t="s">
+        <v>42</v>
+      </c>
+      <c r="C50" s="51" t="s">
+        <v>42</v>
+      </c>
+      <c r="D50" s="52"/>
+      <c r="E50" s="53" t="s">
+        <v>42</v>
+      </c>
+      <c r="F50" s="54" t="s">
+        <v>42</v>
+      </c>
+      <c r="G50" s="24"/>
+      <c r="H50" s="24" t="e">
+        <f t="shared" si="7"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="I50" s="55"/>
+      <c r="J50" s="55"/>
+      <c r="K50" s="55"/>
+      <c r="L50" s="55"/>
+      <c r="M50" s="55"/>
+      <c r="N50" s="55"/>
+      <c r="O50" s="55"/>
+      <c r="P50" s="55"/>
+      <c r="Q50" s="55"/>
+      <c r="R50" s="55"/>
+      <c r="S50" s="55"/>
+      <c r="T50" s="55"/>
+      <c r="U50" s="55"/>
+      <c r="V50" s="55"/>
+      <c r="W50" s="55"/>
+      <c r="X50" s="55"/>
+      <c r="Y50" s="55"/>
+      <c r="Z50" s="55"/>
+      <c r="AA50" s="55"/>
+      <c r="AB50" s="55"/>
+      <c r="AC50" s="55"/>
+      <c r="AD50" s="55"/>
+      <c r="AE50" s="55"/>
+      <c r="AF50" s="55"/>
+      <c r="AG50" s="55"/>
+      <c r="AH50" s="55"/>
+      <c r="AI50" s="55"/>
+      <c r="AJ50" s="55"/>
+      <c r="AK50" s="55"/>
+      <c r="AL50" s="55"/>
+      <c r="AM50" s="55"/>
+      <c r="AN50" s="55"/>
+      <c r="AO50" s="55"/>
+      <c r="AP50" s="55"/>
+      <c r="AQ50" s="55"/>
+      <c r="AR50" s="55"/>
+      <c r="AS50" s="55"/>
+      <c r="AT50" s="55"/>
+      <c r="AU50" s="55"/>
+      <c r="AV50" s="55"/>
+      <c r="AW50" s="55"/>
+      <c r="AX50" s="55"/>
+      <c r="AY50" s="55"/>
+      <c r="AZ50" s="55"/>
+      <c r="BA50" s="55"/>
+      <c r="BB50" s="55"/>
+      <c r="BC50" s="55"/>
+      <c r="BD50" s="55"/>
+      <c r="BE50" s="55"/>
+      <c r="BF50" s="55"/>
+      <c r="BG50" s="55"/>
+      <c r="BH50" s="55"/>
+      <c r="BI50" s="55"/>
+      <c r="BJ50" s="55"/>
+      <c r="BK50" s="55"/>
+      <c r="BL50" s="55"/>
+    </row>
+    <row r="51" spans="1:64" s="3" customFormat="1" ht="21.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A51" s="18"/>
+      <c r="B51" s="50" t="s">
+        <v>42</v>
+      </c>
+      <c r="C51" s="51" t="s">
+        <v>42</v>
+      </c>
+      <c r="D51" s="52"/>
+      <c r="E51" s="53" t="s">
+        <v>42</v>
+      </c>
+      <c r="F51" s="54" t="s">
+        <v>42</v>
+      </c>
+      <c r="G51" s="24"/>
+      <c r="H51" s="24" t="e">
+        <f t="shared" si="7"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="I51" s="55"/>
+      <c r="J51" s="55"/>
+      <c r="K51" s="55"/>
+      <c r="L51" s="55"/>
+      <c r="M51" s="55"/>
+      <c r="N51" s="55"/>
+      <c r="O51" s="55"/>
+      <c r="P51" s="55"/>
+      <c r="Q51" s="55"/>
+      <c r="R51" s="55"/>
+      <c r="S51" s="55"/>
+      <c r="T51" s="55"/>
+      <c r="U51" s="55"/>
+      <c r="V51" s="55"/>
+      <c r="W51" s="55"/>
+      <c r="X51" s="55"/>
+      <c r="Y51" s="55"/>
+      <c r="Z51" s="55"/>
+      <c r="AA51" s="55"/>
+      <c r="AB51" s="55"/>
+      <c r="AC51" s="55"/>
+      <c r="AD51" s="55"/>
+      <c r="AE51" s="55"/>
+      <c r="AF51" s="55"/>
+      <c r="AG51" s="55"/>
+      <c r="AH51" s="55"/>
+      <c r="AI51" s="55"/>
+      <c r="AJ51" s="55"/>
+      <c r="AK51" s="55"/>
+      <c r="AL51" s="55"/>
+      <c r="AM51" s="55"/>
+      <c r="AN51" s="55"/>
+      <c r="AO51" s="55"/>
+      <c r="AP51" s="55"/>
+      <c r="AQ51" s="55"/>
+      <c r="AR51" s="55"/>
+      <c r="AS51" s="55"/>
+      <c r="AT51" s="55"/>
+      <c r="AU51" s="55"/>
+      <c r="AV51" s="55"/>
+      <c r="AW51" s="55"/>
+      <c r="AX51" s="55"/>
+      <c r="AY51" s="55"/>
+      <c r="AZ51" s="55"/>
+      <c r="BA51" s="55"/>
+      <c r="BB51" s="55"/>
+      <c r="BC51" s="55"/>
+      <c r="BD51" s="55"/>
+      <c r="BE51" s="55"/>
+      <c r="BF51" s="55"/>
+      <c r="BG51" s="55"/>
+      <c r="BH51" s="55"/>
+      <c r="BI51" s="55"/>
+      <c r="BJ51" s="55"/>
+      <c r="BK51" s="55"/>
+      <c r="BL51" s="55"/>
+    </row>
+    <row r="52" spans="1:64" x14ac:dyDescent="0.3">
+      <c r="B52" s="72"/>
+      <c r="C52" s="17"/>
+    </row>
+    <row r="53" spans="1:64" x14ac:dyDescent="0.3">
+      <c r="B53" s="71"/>
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="J1:AA1"/>
-    <mergeCell ref="AK4:AQ4"/>
-    <mergeCell ref="AR4:AX4"/>
-    <mergeCell ref="AY4:BE4"/>
-    <mergeCell ref="BF4:BL4"/>
     <mergeCell ref="E2:F2"/>
     <mergeCell ref="I4:O4"/>
     <mergeCell ref="P4:V4"/>
     <mergeCell ref="W4:AC4"/>
     <mergeCell ref="AD4:AJ4"/>
     <mergeCell ref="E3:F3"/>
+    <mergeCell ref="J1:AA1"/>
+    <mergeCell ref="AK4:AQ4"/>
+    <mergeCell ref="AR4:AX4"/>
+    <mergeCell ref="AY4:BE4"/>
+    <mergeCell ref="BF4:BL4"/>
   </mergeCells>
-  <conditionalFormatting sqref="D7:D39">
+  <phoneticPr fontId="26" type="noConversion"/>
+  <conditionalFormatting sqref="D7:D51">
     <cfRule type="dataBar" priority="14">
       <dataBar>
         <cfvo type="num" val="0"/>
@@ -4665,7 +5641,7 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I15:BL39">
+  <conditionalFormatting sqref="I15:BL51">
     <cfRule type="expression" dxfId="4" priority="27">
       <formula>AND(task_start&lt;=I$5,ROUNDDOWN((task_end-task_start+1)*task_progress,0)+task_start-1&gt;=I$5)</formula>
     </cfRule>
@@ -4673,7 +5649,7 @@
       <formula>AND(task_end&gt;=I$5,task_start&lt;I$5+1)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I5:BL39">
+  <conditionalFormatting sqref="I5:BL51">
     <cfRule type="expression" dxfId="2" priority="29">
       <formula>AND(today&gt;=I$5,today&lt;I$5+1)</formula>
     </cfRule>
@@ -4711,7 +5687,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>D7:D39</xm:sqref>
+          <xm:sqref>D7:D51</xm:sqref>
         </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>

</xml_diff>